<commit_message>
Corrige build do sqlite3 no Render
</commit_message>
<xml_diff>
--- a/dados_filtrados.xlsx
+++ b/dados_filtrados.xlsx
@@ -524,17 +524,17 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>C:/Onedrive/EMPRESAS/TERCEIROS/Simples Nacional/P R RAMOS CONSULTORIA CONTABIL/Declarações/2025/SIMPLES NACIONAL\Declaração Mensal_Recibo DAS - API Integra Contador - Empresa 15 - 062025.pdf, C:/Onedrive/EMPRESAS/TERCEIROS/Simples Nacional/P R RAMOS CONSULTORIA CONTABIL/Declarações/2025/SIMPLES NACIONAL\DAS - API Integra Contador - Empresa 15 - 062025.pdf</t>
+          <t>C:/Onedrive/EMPRESAS/TERCEIROS/Diversos/Relatórios a Arquivar/imagem_teste.png</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>simples_nacional</t>
+          <t>Teste</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Olá pessoa_,\nvenho informar, que o imposto/declaração referente ao faturamento do simples nacional do mês mes_ant_ da empresa emp_ foram direcionados no e-mail, \nqualquer duvida estou a disposição</t>
+          <t>Mensagem teste</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">

</xml_diff>